<commit_message>
get lean cloud schema
</commit_message>
<xml_diff>
--- a/testingjs-xlsx/excelData.xlsx
+++ b/testingjs-xlsx/excelData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="106">
   <si>
     <t>最新高校名称</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -294,45 +294,41 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>牛6</t>
+  </si>
+  <si>
+    <t>牛7</t>
+  </si>
+  <si>
+    <t>牛8</t>
+  </si>
+  <si>
+    <t>马1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>马2</t>
+  </si>
+  <si>
+    <t>马3</t>
+  </si>
+  <si>
+    <t>2008年</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>广东外语学院</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>外语学院</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>德语</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>牛6</t>
-  </si>
-  <si>
-    <t>牛7</t>
-  </si>
-  <si>
-    <t>牛8</t>
-  </si>
-  <si>
-    <t>马1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>马2</t>
-  </si>
-  <si>
-    <t>马3</t>
-  </si>
-  <si>
-    <t>2008年</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>广东外语学院</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>外语学院</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>德语</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>马4</t>
   </si>
   <si>
@@ -392,19 +388,57 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>广东外语外贸大学2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>审计1</t>
+  </si>
+  <si>
+    <t>德语1</t>
+  </si>
+  <si>
+    <t>德语3</t>
+  </si>
+  <si>
+    <t>德语4</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>班2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>班3</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -413,14 +447,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -429,7 +463,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -438,7 +472,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -447,10 +481,17 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -497,7 +538,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -513,8 +554,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -534,23 +581,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+  <cellStyles count="21">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -882,7 +941,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -922,7 +981,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>29</v>
@@ -940,11 +999,11 @@
         <v>33</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="H2" s="3" t="str">
         <f>F2&amp;G2</f>
-        <v>审计1班</v>
+        <v>审计1班2</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>35</v>
@@ -952,7 +1011,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -970,11 +1029,11 @@
         <v>11</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
       <c r="H3" s="3" t="str">
         <f t="shared" ref="H3:H12" si="0">F3&amp;G3</f>
-        <v>审计1班</v>
+        <v>审计1班3</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>36</v>
@@ -982,7 +1041,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>38</v>
@@ -1012,7 +1071,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -1042,7 +1101,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
@@ -1072,7 +1131,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -1102,7 +1161,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
@@ -1132,7 +1191,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
@@ -1162,7 +1221,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>38</v>
@@ -1192,7 +1251,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>38</v>
@@ -1222,7 +1281,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>38</v>
@@ -1252,7 +1311,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
@@ -1282,7 +1341,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>38</v>
@@ -1312,7 +1371,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>8</v>
@@ -1342,7 +1401,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>38</v>
@@ -1372,7 +1431,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>61</v>
@@ -1402,7 +1461,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>38</v>
@@ -1432,7 +1491,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>38</v>
@@ -1462,7 +1521,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>69</v>
@@ -1476,23 +1535,23 @@
       <c r="E20" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>73</v>
+      <c r="F20" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H20" s="4" t="str">
         <f>F20&amp;G20</f>
-        <v>德语1班</v>
+        <v>德语41班</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>20</v>
@@ -1506,23 +1565,23 @@
       <c r="E21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>17</v>
+      <c r="F21" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="4" t="str">
         <f t="shared" ref="H21:H30" si="2">F21&amp;G21</f>
-        <v>德语1班</v>
+        <v>德语31班</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>20</v>
@@ -1547,12 +1606,12 @@
         <v>德语1班</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>20</v>
@@ -1577,12 +1636,12 @@
         <v>德语1班</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>20</v>
@@ -1607,12 +1666,12 @@
         <v>德语1班</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>20</v>
@@ -1637,27 +1696,27 @@
         <v>德语1班</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>58</v>
@@ -1667,27 +1726,27 @@
         <v>德语2班</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>58</v>
@@ -1697,27 +1756,27 @@
         <v>德语2班</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>58</v>
@@ -1727,27 +1786,27 @@
         <v>德语2班</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>58</v>
@@ -1757,12 +1816,12 @@
         <v>德语2班</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>20</v>
@@ -1776,26 +1835,26 @@
       <c r="E30" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>17</v>
+      <c r="F30" s="8" t="s">
+        <v>101</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>13</v>
       </c>
       <c r="H30" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>德语2班</v>
+        <v>德语12班</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>51</v>
@@ -1807,7 +1866,7 @@
         <v>24</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>42</v>
@@ -1817,12 +1876,12 @@
         <v>软件工程1班</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>25</v>
@@ -1847,12 +1906,12 @@
         <v>软件工程1班</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>25</v>
@@ -1877,12 +1936,12 @@
         <v>软件工程1班</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>25</v>
@@ -1894,7 +1953,7 @@
         <v>26</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>22</v>
@@ -1907,12 +1966,12 @@
         <v>审计1班</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>25</v>
@@ -1924,7 +1983,7 @@
         <v>26</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>22</v>
@@ -1937,15 +1996,15 @@
         <v>审计1班</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>51</v>
@@ -1954,20 +2013,20 @@
         <v>26</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>22</v>
+        <v>97</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>23</v>
       </c>
       <c r="H36" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>审计1班</v>
+        <v>审计11班</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>